<commit_message>
xog tam phan upload file
</commit_message>
<xml_diff>
--- a/src/Resources/excelFile/DemoDaHuaImport1.xlsx
+++ b/src/Resources/excelFile/DemoDaHuaImport1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NamND\Desktop\DahuaImport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SourceGitHub\dahua_import\src\Resources\excelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3348" yWindow="0" windowWidth="21924" windowHeight="9780"/>
+    <workbookView xWindow="3345" yWindow="0" windowWidth="21930" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,15 +354,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -376,7 +376,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -391,7 +391,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -402,11 +402,11 @@
         <v>1214</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D8" si="0" xml:space="preserve"> B3 - C3</f>
+        <f t="shared" ref="D3:D6" si="0" xml:space="preserve"> B3 - C3</f>
         <v>11198</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -421,7 +421,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -436,49 +436,19 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>4124</v>
+        <v>123</v>
       </c>
       <c r="C6">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>1424</v>
-      </c>
-      <c r="C7">
-        <v>124</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>51231</v>
-      </c>
-      <c r="C8">
-        <v>512</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>50719</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>